<commit_message>
finished grid search for "half cutoff = -1"
</commit_message>
<xml_diff>
--- a/ex1/results/grid search results.xlsx
+++ b/ex1/results/grid search results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Team Watson\Tomer\AMNLP\ex1\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F62BEC7-0C09-427B-89DF-25E1BA28153E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A23E48-BDA0-4DBB-9C03-9760977769A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1340" yWindow="2955" windowWidth="24042" windowHeight="12772" xr2:uid="{59572A83-A88A-4D94-AE9E-C7BB10C5D8F0}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{59572A83-A88A-4D94-AE9E-C7BB10C5D8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
   <si>
     <t>==================================================================================</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>Validation accuracy: 0.561, Training accuracy:0.702</t>
+  </si>
+  <si>
+    <t>Validation accuracy: 0.565, Training accuracy:0.712</t>
+  </si>
+  <si>
+    <t>Validation accuracy: 0.567, Training accuracy:0.719</t>
+  </si>
+  <si>
+    <t>Validation accuracy: 0.558, Training accuracy:0.695</t>
+  </si>
+  <si>
+    <t>Validation accuracy: 0.560, Training accuracy:0.702</t>
+  </si>
+  <si>
+    <t>Validation accuracy: 0.562, Training accuracy:0.706</t>
   </si>
 </sst>
 </file>
@@ -513,7 +528,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:F22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -704,6 +719,12 @@
       <c r="D10" s="3">
         <v>10</v>
       </c>
+      <c r="E10">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="F10">
+        <v>0.71199999999999997</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
@@ -717,6 +738,12 @@
       </c>
       <c r="D11" s="3">
         <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="F11">
+        <v>0.71899999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -875,6 +902,12 @@
       <c r="D20" s="3">
         <v>10</v>
       </c>
+      <c r="E20">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="F20">
+        <v>0.69499999999999995</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
@@ -889,6 +922,12 @@
       <c r="D21" s="3">
         <v>10</v>
       </c>
+      <c r="E21">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F21">
+        <v>0.70199999999999996</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
@@ -902,6 +941,12 @@
       </c>
       <c r="D22" s="3">
         <v>10</v>
+      </c>
+      <c r="E22">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F22">
+        <v>0.70599999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -911,10 +956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2A84F0-06F9-497E-B91D-A630D2B75C4E}">
-  <dimension ref="A1:A67"/>
+  <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1189,6 +1234,101 @@
         <v>37</v>
       </c>
     </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>